<commit_message>
NPC home page uses js to show npcs
</commit_message>
<xml_diff>
--- a/Raw Chars/AllChars.xlsx
+++ b/Raw Chars/AllChars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mace\Desktop\MHA\Raw Chars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B343FD-474D-4830-AB16-B1DC7E0F04BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75360850-ED33-478D-B559-720D0CF0CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E2E4C64-C629-49B1-B665-634009757B23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{8E2E4C64-C629-49B1-B665-634009757B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,280 +532,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4743D5A6-F19D-4D57-8191-C96B284E3CA8}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="I7" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>